<commit_message>
test-3 (more cities in input, w/o constr.
</commit_message>
<xml_diff>
--- a/migforecasting/less100/input prep/moreinputNY.xlsx
+++ b/migforecasting/less100/input prep/moreinputNY.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Сланцы</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -110,13 +116,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +448,7 @@
     <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,11 +479,17 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -506,10 +521,16 @@
         <v>399.8</v>
       </c>
       <c r="K2" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="L2" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="M2" s="2">
         <v>-51</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -541,10 +562,16 @@
         <v>29.247</v>
       </c>
       <c r="K3" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L3" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M3" s="2">
         <v>-76</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -576,10 +603,16 @@
         <v>32.409999999999997</v>
       </c>
       <c r="K4" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L4" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M4" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -611,10 +644,16 @@
         <v>24.484999999999999</v>
       </c>
       <c r="K5" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L5" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M5" s="2">
         <v>-257</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -646,10 +685,16 @@
         <v>16.149000000000001</v>
       </c>
       <c r="K6" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L6" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M6" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -681,10 +726,16 @@
         <v>17.542000000000002</v>
       </c>
       <c r="K7" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L7" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M7" s="2">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -716,10 +767,16 @@
         <v>14.432</v>
       </c>
       <c r="K8" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L8" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M8" s="2">
         <v>-99</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -751,10 +808,16 @@
         <v>358.774</v>
       </c>
       <c r="K9" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L9" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M9" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -786,10 +849,16 @@
         <v>799.875</v>
       </c>
       <c r="K10" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L10" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M10" s="2">
         <v>-39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -821,10 +890,16 @@
         <v>886.95799999999997</v>
       </c>
       <c r="K11" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L11" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M11" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -856,10 +931,16 @@
         <v>136.577</v>
       </c>
       <c r="K12" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="L12" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="M12" s="2">
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -891,10 +972,16 @@
         <v>76.884299999999996</v>
       </c>
       <c r="K13" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L13" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M13" s="2">
         <v>-440</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -926,10 +1013,16 @@
         <v>114.82769999999999</v>
       </c>
       <c r="K14" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L14" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M14" s="2">
         <v>-212</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -961,10 +1054,16 @@
         <v>482.38299999999998</v>
       </c>
       <c r="K15" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L15" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M15" s="2">
         <v>-907</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -996,10 +1095,16 @@
         <v>368.78840000000002</v>
       </c>
       <c r="K16" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L16" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M16" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1031,10 +1136,16 @@
         <v>710.65710000000001</v>
       </c>
       <c r="K17" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L17" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M17" s="2">
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1066,10 +1177,16 @@
         <v>775.67230000000006</v>
       </c>
       <c r="K18" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="L18" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="M18" s="2">
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1101,10 +1218,16 @@
         <v>123.943</v>
       </c>
       <c r="K19" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="L19" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="M19" s="2">
         <v>-114</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1136,10 +1259,16 @@
         <v>130.23500000000001</v>
       </c>
       <c r="K20" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="L20" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="M20" s="2">
         <v>-28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1171,10 +1300,16 @@
         <v>170.054</v>
       </c>
       <c r="K21" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="L21" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="M21" s="2">
         <v>-1280</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1206,10 +1341,16 @@
         <v>119.837</v>
       </c>
       <c r="K22" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="L22" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="M22" s="2">
         <v>942</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1241,10 +1382,16 @@
         <v>722</v>
       </c>
       <c r="K23" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="L23" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="M23" s="2">
         <v>767</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -1276,10 +1423,16 @@
         <v>128.20910000000001</v>
       </c>
       <c r="K24" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="L24" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="M24" s="2">
         <v>-63</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -1311,10 +1464,16 @@
         <v>132.601</v>
       </c>
       <c r="K25" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="M25" s="2">
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -1346,10 +1505,16 @@
         <v>171.5384</v>
       </c>
       <c r="K26" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="L26" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="M26" s="2">
         <v>-3761</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1381,10 +1546,16 @@
         <v>290</v>
       </c>
       <c r="K27" s="2">
+        <v>59.07</v>
+      </c>
+      <c r="L27" s="2">
+        <v>28.05</v>
+      </c>
+      <c r="M27" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>

</xml_diff>